<commit_message>
Init Subcooled Solver and File Directories
</commit_message>
<xml_diff>
--- a/RegenSolver/enginefiles/channeltable.xlsx
+++ b/RegenSolver/enginefiles/channeltable.xlsx
@@ -408,7 +408,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>19.53420575792329</v>
+        <v>22.43773118810929</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -416,7 +416,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6.694138511583735</v>
+        <v>2.100966953615222</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -424,7 +424,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>35.92153710833688</v>
+        <v>34.49896502285155</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -432,7 +432,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>